<commit_message>
Bug fixes - extended MS timeout timer to 32 bits to cope with 100,000 - fixed color lookup in 16/16 color mode - length of the word SCREENPLACE Added new FORTH words - COUNTER, returns count of rolling 32 bit MS counter - SEVENSEG, writes a value to the Nexys seven-segment display
</commit_message>
<xml_diff>
--- a/Resources/VGA timing.xlsx
+++ b/Resources/VGA timing.xlsx
@@ -419,7 +419,7 @@
   <dimension ref="A3:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:I15"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -489,7 +489,7 @@
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -518,7 +518,7 @@
       </c>
       <c r="I6">
         <f>I5+D6</f>
-        <v>1190</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -573,7 +573,7 @@
         <v>5</v>
       </c>
       <c r="I8">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:9">

</xml_diff>

<commit_message>
Updated EDITOR.F and system documentation
</commit_message>
<xml_diff>
--- a/Resources/VGA timing.xlsx
+++ b/Resources/VGA timing.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Visible area</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>ROWS / COLS settings</t>
-  </si>
-  <si>
-    <t>WORKS</t>
   </si>
 </sst>
 </file>
@@ -196,7 +193,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -206,6 +203,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,14 +511,15 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E17" sqref="B15:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -575,7 +576,7 @@
       </c>
       <c r="E4">
         <f>E14</f>
-        <v>2500</v>
+        <v>2592</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -613,7 +614,7 @@
       </c>
       <c r="E6" s="2">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>57.870370370370374</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -634,16 +635,14 @@
       </c>
       <c r="E7" s="2">
         <f t="shared" si="2"/>
-        <v>52.863436123348016</v>
+        <v>50.987110458476096</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F9" t="s">
-        <v>41</v>
-      </c>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -661,9 +660,6 @@
       <c r="E10">
         <v>1920</v>
       </c>
-      <c r="F10">
-        <v>1920</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -679,9 +675,6 @@
         <v>24</v>
       </c>
       <c r="E11">
-        <v>50</v>
-      </c>
-      <c r="F11">
         <v>128</v>
       </c>
     </row>
@@ -699,9 +692,6 @@
         <v>136</v>
       </c>
       <c r="E12">
-        <v>150</v>
-      </c>
-      <c r="F12">
         <v>350</v>
       </c>
     </row>
@@ -722,9 +712,6 @@
         <v>144</v>
       </c>
       <c r="E13">
-        <v>148</v>
-      </c>
-      <c r="F13">
         <v>194</v>
       </c>
     </row>
@@ -742,66 +729,27 @@
         <v>1328</v>
       </c>
       <c r="E14">
-        <v>2500</v>
-      </c>
-      <c r="F14">
         <v>2592</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="5">
-        <f>B12/B6</f>
-        <v>3.0720000000000001</v>
-      </c>
-      <c r="C15" s="5">
-        <f t="shared" ref="C15:E15" si="4">C12/C6</f>
-        <v>2.496</v>
-      </c>
-      <c r="D15" s="5">
-        <f t="shared" si="4"/>
-        <v>2.4081066666666664</v>
-      </c>
-      <c r="E15" s="5">
-        <f t="shared" si="4"/>
-        <v>2.5</v>
-      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="5">
-        <f>B14/B10</f>
-        <v>1.25</v>
-      </c>
-      <c r="C16" s="5">
-        <f t="shared" ref="C16:E16" si="5">C14/C10</f>
-        <v>1.3</v>
-      </c>
-      <c r="D16" s="5">
-        <f t="shared" si="5"/>
-        <v>1.296875</v>
-      </c>
-      <c r="E16" s="5">
-        <f t="shared" si="5"/>
-        <v>1.3020833333333333</v>
-      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
-        <f>B11/B10</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C17" s="6">
-        <f>C11/C10</f>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D17" s="6">
-        <f>D11/D10</f>
-        <v>2.34375E-2</v>
-      </c>
-      <c r="E17" s="6">
-        <f>E11/E10</f>
-        <v>2.6041666666666668E-2</v>
-      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -870,15 +818,15 @@
         <v>35</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:E22" si="6">C23-SUM(C19:C21)</f>
+        <f t="shared" ref="C22:E22" si="4">C23-SUM(C19:C21)</f>
         <v>23</v>
       </c>
       <c r="D22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="E22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>51</v>
       </c>
     </row>
@@ -891,15 +839,15 @@
         <v>527</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:E23" si="7">C5</f>
+        <f t="shared" ref="C23:E23" si="5">C5</f>
         <v>666</v>
       </c>
       <c r="D23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>806</v>
       </c>
       <c r="E23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1135</v>
       </c>
     </row>
@@ -930,7 +878,7 @@
       </c>
       <c r="E26">
         <f>E14-1</f>
-        <v>2499</v>
+        <v>2591</v>
       </c>
       <c r="G26" t="s">
         <v>20</v>
@@ -954,7 +902,7 @@
       </c>
       <c r="E27">
         <f>E10+E11+E30</f>
-        <v>1970</v>
+        <v>2048</v>
       </c>
       <c r="G27" t="s">
         <v>21</v>
@@ -978,7 +926,7 @@
       </c>
       <c r="E28">
         <f>E27+E12</f>
-        <v>2120</v>
+        <v>2398</v>
       </c>
       <c r="G28" t="s">
         <v>22</v>
@@ -1130,15 +1078,15 @@
         <v>526</v>
       </c>
       <c r="C36">
-        <f t="shared" ref="C36:D36" si="8">C32-1</f>
+        <f t="shared" ref="C36:D36" si="6">C32-1</f>
         <v>665</v>
       </c>
       <c r="D36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>805</v>
       </c>
       <c r="E36">
-        <f t="shared" ref="E36" si="9">E32-1</f>
+        <f t="shared" ref="E36" si="7">E32-1</f>
         <v>1134</v>
       </c>
       <c r="G36" t="s">

</xml_diff>

<commit_message>
Working and tested simplified VGA controller and text buffer
</commit_message>
<xml_diff>
--- a/Resources/VGA timing.xlsx
+++ b/Resources/VGA timing.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Visible area</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Vd</t>
   </si>
   <si>
-    <t>Ve</t>
-  </si>
-  <si>
     <t>last horizontal pixel on the full line</t>
   </si>
   <si>
@@ -99,12 +96,6 @@
     <t>end of vertical front porch (Vsync ends)</t>
   </si>
   <si>
-    <t>last but one visible vertical pixel</t>
-  </si>
-  <si>
-    <t>last vertical pixel less one</t>
-  </si>
-  <si>
     <t>Whole line (pixels)</t>
   </si>
   <si>
@@ -139,6 +130,12 @@
   </si>
   <si>
     <t>ROWS / COLS settings</t>
+  </si>
+  <si>
+    <t>pre-fetch offset</t>
+  </si>
+  <si>
+    <t>last visible vertical pixel</t>
   </si>
 </sst>
 </file>
@@ -146,7 +143,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -202,7 +199,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -508,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="B15:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,16 +521,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -560,7 +557,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <f>B14</f>
@@ -581,7 +578,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>527</v>
@@ -598,7 +595,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2">
         <f>B3*1000/B4</f>
@@ -619,7 +616,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2">
         <f>1000*B6/B5</f>
@@ -856,7 +853,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E25"/>
     </row>
@@ -881,7 +878,7 @@
         <v>2591</v>
       </c>
       <c r="G26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -905,7 +902,7 @@
         <v>2048</v>
       </c>
       <c r="G27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -929,7 +926,7 @@
         <v>2398</v>
       </c>
       <c r="G28" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -953,7 +950,7 @@
         <v>1919</v>
       </c>
       <c r="G29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -978,23 +975,23 @@
         <v>15</v>
       </c>
       <c r="B32">
-        <f>B23</f>
+        <f>B23-B38</f>
         <v>527</v>
       </c>
       <c r="C32">
-        <f>C23</f>
+        <f t="shared" ref="C32:E32" si="6">C23-C38</f>
         <v>666</v>
       </c>
       <c r="D32">
-        <f>D23</f>
+        <f t="shared" si="6"/>
         <v>806</v>
       </c>
       <c r="E32">
-        <f>E23</f>
+        <f t="shared" si="6"/>
         <v>1135</v>
       </c>
       <c r="G32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1014,11 +1011,10 @@
         <v>771</v>
       </c>
       <c r="E33">
-        <f>E19+E20+E37</f>
-        <v>1081</v>
+        <v>1086</v>
       </c>
       <c r="G33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1038,11 +1034,10 @@
         <v>777</v>
       </c>
       <c r="E34">
-        <f>E33+E21</f>
-        <v>1084</v>
+        <v>1094</v>
       </c>
       <c r="G34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1050,48 +1045,28 @@
         <v>18</v>
       </c>
       <c r="B35">
-        <f>B19-2</f>
-        <v>478</v>
+        <f>B19-1-B38</f>
+        <v>479</v>
       </c>
       <c r="C35">
-        <f>C19-2</f>
-        <v>598</v>
+        <f t="shared" ref="C35:E35" si="7">C19-1-C38</f>
+        <v>599</v>
       </c>
       <c r="D35">
-        <f>D19-2</f>
-        <v>766</v>
+        <f t="shared" si="7"/>
+        <v>767</v>
       </c>
       <c r="E35">
-        <f>E19-2</f>
-        <v>1078</v>
+        <f t="shared" si="7"/>
+        <v>1079</v>
       </c>
       <c r="G35" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36">
-        <f>B32-1</f>
-        <v>526</v>
-      </c>
-      <c r="C36">
-        <f t="shared" ref="C36:D36" si="6">C32-1</f>
-        <v>665</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="6"/>
-        <v>805</v>
-      </c>
-      <c r="E36">
-        <f t="shared" ref="E36" si="7">E32-1</f>
-        <v>1134</v>
-      </c>
-      <c r="G36" t="s">
-        <v>28</v>
-      </c>
+      <c r="A36" s="4"/>
+      <c r="E36"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
@@ -1110,70 +1085,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>40</v>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>9</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <f>B10/8</f>
         <v>80</v>
       </c>
-      <c r="C40">
+      <c r="C41">
         <f>C10/8</f>
         <v>100</v>
       </c>
-      <c r="D40">
+      <c r="D41">
         <f>D10/8</f>
         <v>128</v>
       </c>
-      <c r="E40">
+      <c r="E41">
         <f>E10/8</f>
         <v>240</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>33</v>
-      </c>
-      <c r="B41">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42">
         <f>B19/8</f>
         <v>60</v>
       </c>
-      <c r="C41">
+      <c r="C42">
         <f>C19/8</f>
         <v>75</v>
       </c>
-      <c r="D41">
+      <c r="D42">
         <f>D19/8</f>
         <v>96</v>
       </c>
-      <c r="E41">
+      <c r="E42">
         <f>E19/8</f>
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B42">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43">
         <f>ROUNDDOWN(B19/10,0)</f>
         <v>48</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <f>ROUNDDOWN(C19/10,0)</f>
         <v>60</v>
       </c>
-      <c r="D42">
+      <c r="D43">
         <f>ROUNDDOWN(D19/10,0)</f>
         <v>76</v>
       </c>
-      <c r="E42">
+      <c r="E43">
         <f>ROUNDDOWN(E19/10,0)</f>
         <v>108</v>
       </c>

</xml_diff>

<commit_message>
Fix bug with missing top row
</commit_message>
<xml_diff>
--- a/Resources/VGA timing.xlsx
+++ b/Resources/VGA timing.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Visible area</t>
   </si>
@@ -132,10 +132,10 @@
     <t>ROWS / COLS settings</t>
   </si>
   <si>
-    <t>pre-fetch offset</t>
-  </si>
-  <si>
     <t>last visible vertical pixel</t>
+  </si>
+  <si>
+    <t>Whole screen</t>
   </si>
 </sst>
 </file>
@@ -190,7 +190,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -198,11 +198,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,18 +502,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
     <col min="2" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="5" max="6" width="12.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -532,6 +528,7 @@
       <c r="E1" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -554,6 +551,7 @@
       <c r="E3">
         <v>150</v>
       </c>
+      <c r="F3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -575,6 +573,7 @@
         <f>E14</f>
         <v>2592</v>
       </c>
+      <c r="F4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -592,6 +591,7 @@
       <c r="E5">
         <v>1135</v>
       </c>
+      <c r="F5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -613,6 +613,7 @@
         <f t="shared" si="1"/>
         <v>57.870370370370374</v>
       </c>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -634,12 +635,12 @@
         <f t="shared" si="2"/>
         <v>50.987110458476096</v>
       </c>
+      <c r="F7" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -657,6 +658,7 @@
       <c r="E10">
         <v>1920</v>
       </c>
+      <c r="F10"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -674,6 +676,7 @@
       <c r="E11">
         <v>128</v>
       </c>
+      <c r="F11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -691,6 +694,7 @@
       <c r="E12">
         <v>350</v>
       </c>
+      <c r="F12"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -711,6 +715,7 @@
       <c r="E13">
         <v>194</v>
       </c>
+      <c r="F13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -728,447 +733,487 @@
       <c r="E14">
         <v>2592</v>
       </c>
+      <c r="F14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="G17" s="1"/>
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>480</v>
+      </c>
+      <c r="C17">
+        <v>600</v>
+      </c>
+      <c r="D17">
+        <v>768</v>
+      </c>
+      <c r="E17">
+        <v>1080</v>
+      </c>
+      <c r="F17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>37</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <f>-6+12</f>
         <v>6</v>
       </c>
-      <c r="G18" s="1"/>
+      <c r="F18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B19">
-        <v>480</v>
+        <v>2</v>
       </c>
       <c r="C19">
-        <v>600</v>
+        <v>6</v>
       </c>
       <c r="D19">
-        <v>768</v>
+        <v>6</v>
       </c>
       <c r="E19">
-        <v>1080</v>
-      </c>
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="F19"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B20">
-        <v>10</v>
+        <f>B21-SUM(B17:B19)</f>
+        <v>35</v>
       </c>
       <c r="C20">
-        <v>37</v>
+        <f t="shared" ref="C20:E20" si="4">C21-SUM(C17:C19)</f>
+        <v>23</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>29</v>
       </c>
       <c r="E20">
-        <v>1</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="F20"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21">
-        <v>6</v>
-      </c>
-      <c r="D21">
-        <v>6</v>
-      </c>
-      <c r="E21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22">
-        <f>B23-SUM(B19:B21)</f>
-        <v>35</v>
-      </c>
-      <c r="C22">
-        <f t="shared" ref="C22:E22" si="4">C23-SUM(C19:C21)</f>
-        <v>23</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="4"/>
-        <v>29</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="4"/>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23">
         <f>B5</f>
         <v>527</v>
       </c>
-      <c r="C23">
-        <f t="shared" ref="C23:E23" si="5">C5</f>
+      <c r="C21">
+        <f>C5</f>
         <v>666</v>
       </c>
-      <c r="D23">
+      <c r="D21">
+        <f>D5</f>
+        <v>806</v>
+      </c>
+      <c r="E21">
+        <f>E5</f>
+        <v>1135</v>
+      </c>
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22"/>
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23"/>
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <f>B14-1</f>
+        <v>799</v>
+      </c>
+      <c r="C24">
+        <f>C14-1</f>
+        <v>1039</v>
+      </c>
+      <c r="D24">
+        <f>D14-1</f>
+        <v>1327</v>
+      </c>
+      <c r="E24">
+        <f>E14-1</f>
+        <v>2591</v>
+      </c>
+      <c r="F24"/>
+      <c r="G24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25">
+        <f>B10+B11+B28</f>
+        <v>656</v>
+      </c>
+      <c r="C25">
+        <f>C10+C11+C28</f>
+        <v>856</v>
+      </c>
+      <c r="D25">
+        <f>D10+D11+D28</f>
+        <v>1048</v>
+      </c>
+      <c r="E25">
+        <f>E10+E11+E28</f>
+        <v>2048</v>
+      </c>
+      <c r="F25"/>
+      <c r="G25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26">
+        <f>B25+B12</f>
+        <v>752</v>
+      </c>
+      <c r="C26">
+        <f>C25+C12</f>
+        <v>976</v>
+      </c>
+      <c r="D26">
+        <f>D25+D12</f>
+        <v>1184</v>
+      </c>
+      <c r="E26">
+        <f>E25+E12</f>
+        <v>2398</v>
+      </c>
+      <c r="F26"/>
+      <c r="G26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27">
+        <f>B10-1</f>
+        <v>639</v>
+      </c>
+      <c r="C27">
+        <f>C10-1</f>
+        <v>799</v>
+      </c>
+      <c r="D27">
+        <f>D10-1</f>
+        <v>1023</v>
+      </c>
+      <c r="E27">
+        <f>E10-1</f>
+        <v>1919</v>
+      </c>
+      <c r="F27"/>
+      <c r="G27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30">
+        <f>B21</f>
+        <v>527</v>
+      </c>
+      <c r="C30">
+        <f t="shared" ref="C30:E30" si="5">C21</f>
+        <v>666</v>
+      </c>
+      <c r="D30">
         <f t="shared" si="5"/>
         <v>806</v>
       </c>
-      <c r="E23">
+      <c r="E30">
         <f t="shared" si="5"/>
         <v>1135</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E24"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26">
-        <f>B14-1</f>
-        <v>799</v>
-      </c>
-      <c r="C26">
-        <f>C14-1</f>
-        <v>1039</v>
-      </c>
-      <c r="D26">
-        <f>D14-1</f>
-        <v>1327</v>
-      </c>
-      <c r="E26">
-        <f>E14-1</f>
-        <v>2591</v>
-      </c>
-      <c r="G26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27">
-        <f>B10+B11+B30</f>
-        <v>656</v>
-      </c>
-      <c r="C27">
-        <f>C10+C11+C30</f>
-        <v>856</v>
-      </c>
-      <c r="D27">
-        <f>D10+D11+D30</f>
-        <v>1048</v>
-      </c>
-      <c r="E27">
-        <f>E10+E11+E30</f>
-        <v>2048</v>
-      </c>
-      <c r="G27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28">
-        <f>B27+B12</f>
-        <v>752</v>
-      </c>
-      <c r="C28">
-        <f>C27+C12</f>
-        <v>976</v>
-      </c>
-      <c r="D28">
-        <f>D27+D12</f>
-        <v>1184</v>
-      </c>
-      <c r="E28">
-        <f>E27+E12</f>
-        <v>2398</v>
-      </c>
-      <c r="G28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29">
-        <f>B10-1</f>
-        <v>639</v>
-      </c>
-      <c r="C29">
-        <f>C10-1</f>
-        <v>799</v>
-      </c>
-      <c r="D29">
-        <f>D10-1</f>
-        <v>1023</v>
-      </c>
-      <c r="E29">
-        <f>E10-1</f>
-        <v>1919</v>
-      </c>
-      <c r="G29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
+      <c r="F30">
+        <v>1135</v>
+      </c>
+      <c r="G30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <f>B17+B18</f>
+        <v>490</v>
+      </c>
+      <c r="C31">
+        <f>C17+C18</f>
+        <v>637</v>
+      </c>
+      <c r="D31">
+        <f>D17+D18</f>
+        <v>771</v>
+      </c>
+      <c r="E31">
+        <f>E17+E18</f>
+        <v>1086</v>
+      </c>
+      <c r="F31">
+        <v>1086</v>
+      </c>
+      <c r="G31" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B32">
-        <f>B23-B38</f>
-        <v>527</v>
+        <f>B31+B19</f>
+        <v>492</v>
       </c>
       <c r="C32">
-        <f t="shared" ref="C32:E32" si="6">C23-C38</f>
-        <v>666</v>
+        <f>C31+C19</f>
+        <v>643</v>
       </c>
       <c r="D32">
-        <f t="shared" si="6"/>
-        <v>806</v>
+        <f>D31+D19</f>
+        <v>777</v>
       </c>
       <c r="E32">
-        <f t="shared" si="6"/>
-        <v>1135</v>
+        <f>E31+E19</f>
+        <v>1094</v>
+      </c>
+      <c r="F32">
+        <v>1094</v>
       </c>
       <c r="G32" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B33">
-        <f>B19+B20+B37</f>
-        <v>490</v>
+        <f>B17-1</f>
+        <v>479</v>
       </c>
       <c r="C33">
-        <f>C19+C20+C37</f>
-        <v>637</v>
+        <f t="shared" ref="C33:E33" si="6">C17-1</f>
+        <v>599</v>
       </c>
       <c r="D33">
-        <f>D19+D20+D37</f>
-        <v>771</v>
+        <f t="shared" si="6"/>
+        <v>767</v>
       </c>
       <c r="E33">
-        <v>1086</v>
+        <f t="shared" si="6"/>
+        <v>1079</v>
+      </c>
+      <c r="F33">
+        <v>1079</v>
       </c>
       <c r="G33" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34">
-        <f>B33+B21</f>
-        <v>492</v>
-      </c>
-      <c r="C34">
-        <f>C33+C21</f>
-        <v>643</v>
-      </c>
-      <c r="D34">
-        <f>D33+D21</f>
-        <v>777</v>
-      </c>
-      <c r="E34">
-        <v>1094</v>
-      </c>
-      <c r="G34" t="s">
-        <v>25</v>
-      </c>
+      <c r="A34" s="4"/>
+      <c r="E34"/>
+      <c r="F34"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35">
-        <f>B19-1-B38</f>
-        <v>479</v>
-      </c>
-      <c r="C35">
-        <f t="shared" ref="C35:E35" si="7">C19-1-C38</f>
-        <v>599</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="7"/>
-        <v>767</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="7"/>
-        <v>1079</v>
-      </c>
-      <c r="G35" t="s">
-        <v>39</v>
+      <c r="A35" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="E36"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A36" t="s">
         <v>9</v>
       </c>
-      <c r="B41">
+      <c r="B36">
         <f>B10/8</f>
         <v>80</v>
       </c>
-      <c r="C41">
+      <c r="C36">
         <f>C10/8</f>
         <v>100</v>
       </c>
-      <c r="D41">
+      <c r="D36">
         <f>D10/8</f>
         <v>128</v>
       </c>
-      <c r="E41">
+      <c r="E36">
         <f>E10/8</f>
         <v>240</v>
       </c>
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37">
+        <f>B17/8</f>
+        <v>60</v>
+      </c>
+      <c r="C37">
+        <f>C17/8</f>
+        <v>75</v>
+      </c>
+      <c r="D37">
+        <f>D17/8</f>
+        <v>96</v>
+      </c>
+      <c r="E37">
+        <f>E17/8</f>
+        <v>135</v>
+      </c>
+      <c r="F37"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38">
+        <f>ROUNDDOWN(B17/10,0)</f>
+        <v>48</v>
+      </c>
+      <c r="C38">
+        <f>ROUNDDOWN(C17/10,0)</f>
+        <v>60</v>
+      </c>
+      <c r="D38">
+        <f>ROUNDDOWN(D17/10,0)</f>
+        <v>76</v>
+      </c>
+      <c r="E38">
+        <f>ROUNDDOWN(E17/10,0)</f>
+        <v>108</v>
+      </c>
+      <c r="F38"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>30</v>
-      </c>
-      <c r="B42">
-        <f>B19/8</f>
-        <v>60</v>
-      </c>
-      <c r="C42">
-        <f>C19/8</f>
-        <v>75</v>
-      </c>
-      <c r="D42">
-        <f>D19/8</f>
-        <v>96</v>
-      </c>
-      <c r="E42">
-        <f>E19/8</f>
-        <v>135</v>
-      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>31</v>
-      </c>
-      <c r="B43">
-        <f>ROUNDDOWN(B19/10,0)</f>
-        <v>48</v>
-      </c>
-      <c r="C43">
-        <f>ROUNDDOWN(C19/10,0)</f>
-        <v>60</v>
-      </c>
-      <c r="D43">
-        <f>ROUNDDOWN(D19/10,0)</f>
-        <v>76</v>
-      </c>
-      <c r="E43">
-        <f>ROUNDDOWN(E19/10,0)</f>
-        <v>108</v>
-      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improvements to VGA timing
</commit_message>
<xml_diff>
--- a/Resources/VGA timing.xlsx
+++ b/Resources/VGA timing.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\N.I.G.E.-Machine\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="375" windowWidth="19875" windowHeight="12300"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -141,11 +146,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +167,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -190,7 +203,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -200,6 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -210,6 +224,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -258,7 +275,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -291,9 +308,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,6 +360,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -505,7 +556,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +631,7 @@
         <v>27</v>
       </c>
       <c r="B5">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C5">
         <v>666</v>
@@ -589,7 +640,7 @@
         <v>806</v>
       </c>
       <c r="E5">
-        <v>1135</v>
+        <v>1125</v>
       </c>
       <c r="F5"/>
     </row>
@@ -621,7 +672,7 @@
       </c>
       <c r="B7" s="2">
         <f>1000*B6/B5</f>
-        <v>59.297912713472485</v>
+        <v>59.523809523809526</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" ref="C7:E7" si="2">1000*C6/C5</f>
@@ -633,7 +684,7 @@
       </c>
       <c r="E7" s="2">
         <f t="shared" si="2"/>
-        <v>50.987110458476096</v>
+        <v>51.440329218106996</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -781,8 +832,7 @@
         <v>3</v>
       </c>
       <c r="E18">
-        <f>-6+12</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F18"/>
     </row>
@@ -800,8 +850,7 @@
         <v>6</v>
       </c>
       <c r="E19">
-        <f>8</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F19"/>
     </row>
@@ -810,11 +859,11 @@
         <v>3</v>
       </c>
       <c r="B20">
-        <f>B21-SUM(B17:B19)</f>
-        <v>35</v>
+        <f t="shared" ref="B20:E20" si="4">B21-SUM(B17:B19)</f>
+        <v>33</v>
       </c>
       <c r="C20">
-        <f t="shared" ref="C20:E20" si="4">C21-SUM(C17:C19)</f>
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
       <c r="D20">
@@ -823,7 +872,7 @@
       </c>
       <c r="E20">
         <f t="shared" si="4"/>
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F20"/>
     </row>
@@ -833,7 +882,7 @@
       </c>
       <c r="B21">
         <f>B5</f>
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C21">
         <f>C5</f>
@@ -845,7 +894,7 @@
       </c>
       <c r="E21">
         <f>E5</f>
-        <v>1135</v>
+        <v>1125</v>
       </c>
       <c r="F21"/>
     </row>
@@ -960,23 +1009,22 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="7">
         <v>0</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="7">
         <v>0</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="7">
         <v>0</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="7">
         <v>0</v>
       </c>
-      <c r="F28"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
@@ -984,7 +1032,7 @@
       </c>
       <c r="B30">
         <f>B21</f>
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C30">
         <f t="shared" ref="C30:E30" si="5">C21</f>
@@ -996,7 +1044,7 @@
       </c>
       <c r="E30">
         <f t="shared" si="5"/>
-        <v>1135</v>
+        <v>1125</v>
       </c>
       <c r="F30">
         <v>1135</v>
@@ -1023,7 +1071,7 @@
       </c>
       <c r="E31">
         <f>E17+E18</f>
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="F31">
         <v>1086</v>
@@ -1050,7 +1098,7 @@
       </c>
       <c r="E32">
         <f>E31+E19</f>
-        <v>1094</v>
+        <v>1089</v>
       </c>
       <c r="F32">
         <v>1094</v>
@@ -1217,7 +1265,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Corrected longstanding problem with VSync and HSync being generated at the wrong part of the scan cycles. Now need to reset pixel generators to match new format
</commit_message>
<xml_diff>
--- a/Resources/VGA timing.xlsx
+++ b/Resources/VGA timing.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16828"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\N.I.G.E.-Machine\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC538E6-06F8-4909-B5CE-78C91C3E99D5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="375" windowWidth="19875" windowHeight="12300"/>
+    <workbookView xWindow="600" yWindow="375" windowWidth="19875" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Visible area</t>
   </si>
@@ -65,9 +66,6 @@
     <t>Hd</t>
   </si>
   <si>
-    <t>offset</t>
-  </si>
-  <si>
     <t>Va</t>
   </si>
   <si>
@@ -80,27 +78,6 @@
     <t>Vd</t>
   </si>
   <si>
-    <t>last horizontal pixel on the full line</t>
-  </si>
-  <si>
-    <t>beginning of horizontal front porch (Hsync begins)</t>
-  </si>
-  <si>
-    <t>end of horizontal front porch (Hsync ends)</t>
-  </si>
-  <si>
-    <t>last visible horizontal pixel</t>
-  </si>
-  <si>
-    <t>last vertical pixel on the full screen</t>
-  </si>
-  <si>
-    <t>beginning of vertical front porch (Vsync begins)</t>
-  </si>
-  <si>
-    <t>end of vertical front porch (Vsync ends)</t>
-  </si>
-  <si>
     <t>Whole line (pixels)</t>
   </si>
   <si>
@@ -135,9 +112,6 @@
   </si>
   <si>
     <t>ROWS / COLS settings</t>
-  </si>
-  <si>
-    <t>last visible vertical pixel</t>
   </si>
   <si>
     <t>Whole screen</t>
@@ -146,11 +120,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,14 +141,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -203,7 +169,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -213,7 +179,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,11 +517,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,16 +533,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F1" s="3"/>
     </row>
@@ -606,7 +571,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <f>B14</f>
@@ -628,7 +593,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>525</v>
@@ -646,7 +611,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2">
         <f>B3*1000/B4</f>
@@ -668,7 +633,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2">
         <f>1000*B6/B5</f>
@@ -787,364 +752,319 @@
       <c r="F14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="1"/>
+      <c r="E15"/>
+      <c r="F15"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <v>480</v>
-      </c>
-      <c r="C17">
-        <v>600</v>
-      </c>
-      <c r="D17">
-        <v>768</v>
-      </c>
-      <c r="E17">
-        <v>1080</v>
-      </c>
-      <c r="F17"/>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18">
-        <v>10</v>
+        <v>480</v>
       </c>
       <c r="C18">
-        <v>37</v>
+        <v>600</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>768</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>1080</v>
       </c>
       <c r="F18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C19">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F19"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>3</v>
       </c>
-      <c r="B20">
-        <f t="shared" ref="B20:E20" si="4">B21-SUM(B17:B19)</f>
+      <c r="B21">
+        <f t="shared" ref="B21:E21" si="4">B22-SUM(B18:B20)</f>
         <v>33</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <f t="shared" si="4"/>
         <v>29</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <f t="shared" si="4"/>
         <v>36</v>
       </c>
-      <c r="F20"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21">
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
         <f>B5</f>
         <v>525</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <f>C5</f>
         <v>666</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <f>D5</f>
         <v>806</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <f>E5</f>
         <v>1125</v>
       </c>
-      <c r="F21"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E22"/>
       <c r="F22"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E23"/>
       <c r="F23"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24"/>
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B24">
+      <c r="B25">
+        <f>B12-1</f>
+        <v>95</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:E25" si="5">C12-1</f>
+        <v>119</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="5"/>
+        <v>135</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="5"/>
+        <v>349</v>
+      </c>
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26">
+        <f>B14-B11-B10-1</f>
+        <v>143</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:E26" si="6">C14-C11-C10-1</f>
+        <v>183</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="6"/>
+        <v>279</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="6"/>
+        <v>543</v>
+      </c>
+      <c r="F26"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <f>B14-B11-1</f>
+        <v>783</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ref="C27:E27" si="7">C14-C11-1</f>
+        <v>983</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="7"/>
+        <v>1303</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="7"/>
+        <v>2463</v>
+      </c>
+      <c r="F27"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
         <f>B14-1</f>
         <v>799</v>
       </c>
-      <c r="C24">
-        <f>C14-1</f>
+      <c r="C28">
+        <f t="shared" ref="C28:E28" si="8">C14-1</f>
         <v>1039</v>
       </c>
-      <c r="D24">
-        <f>D14-1</f>
+      <c r="D28">
+        <f t="shared" si="8"/>
         <v>1327</v>
       </c>
-      <c r="E24">
-        <f>E14-1</f>
+      <c r="E28">
+        <f t="shared" si="8"/>
         <v>2591</v>
       </c>
-      <c r="F24"/>
-      <c r="G24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25">
-        <f>B10+B11+B28</f>
-        <v>656</v>
-      </c>
-      <c r="C25">
-        <f>C10+C11+C28</f>
-        <v>856</v>
-      </c>
-      <c r="D25">
-        <f>D10+D11+D28</f>
-        <v>1048</v>
-      </c>
-      <c r="E25">
-        <f>E10+E11+E28</f>
-        <v>2048</v>
-      </c>
-      <c r="F25"/>
-      <c r="G25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26">
-        <f>B25+B12</f>
-        <v>752</v>
-      </c>
-      <c r="C26">
-        <f>C25+C12</f>
-        <v>976</v>
-      </c>
-      <c r="D26">
-        <f>D25+D12</f>
-        <v>1184</v>
-      </c>
-      <c r="E26">
-        <f>E25+E12</f>
-        <v>2398</v>
-      </c>
-      <c r="F26"/>
-      <c r="G26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27">
-        <f>B10-1</f>
-        <v>639</v>
-      </c>
-      <c r="C27">
-        <f>C10-1</f>
-        <v>799</v>
-      </c>
-      <c r="D27">
-        <f>D10-1</f>
-        <v>1023</v>
-      </c>
-      <c r="E27">
-        <f>E10-1</f>
-        <v>1919</v>
-      </c>
-      <c r="F27"/>
-      <c r="G27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="7">
-        <v>0</v>
-      </c>
-      <c r="C28" s="7">
-        <v>0</v>
-      </c>
-      <c r="D28" s="7">
-        <v>0</v>
-      </c>
-      <c r="E28" s="7">
-        <v>0</v>
-      </c>
+      <c r="F28"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30">
-        <f>B21</f>
-        <v>525</v>
+        <f>B20-1</f>
+        <v>1</v>
       </c>
       <c r="C30">
-        <f t="shared" ref="C30:E30" si="5">C21</f>
-        <v>666</v>
+        <f t="shared" ref="C30:E30" si="9">C20-1</f>
+        <v>5</v>
       </c>
       <c r="D30">
-        <f t="shared" si="5"/>
-        <v>806</v>
+        <f t="shared" si="9"/>
+        <v>5</v>
       </c>
       <c r="E30">
-        <f t="shared" si="5"/>
-        <v>1125</v>
-      </c>
-      <c r="F30">
-        <v>1135</v>
-      </c>
-      <c r="G30" t="s">
-        <v>23</v>
-      </c>
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="F30"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31">
-        <f>B17+B18</f>
-        <v>490</v>
+        <f>B22-B19-B18-1</f>
+        <v>34</v>
       </c>
       <c r="C31">
-        <f>C17+C18</f>
-        <v>637</v>
+        <f t="shared" ref="C31:E31" si="10">C22-C19-C18-1</f>
+        <v>28</v>
       </c>
       <c r="D31">
-        <f>D17+D18</f>
-        <v>771</v>
+        <f t="shared" si="10"/>
+        <v>34</v>
       </c>
       <c r="E31">
-        <f>E17+E18</f>
-        <v>1084</v>
-      </c>
-      <c r="F31">
-        <v>1086</v>
-      </c>
-      <c r="G31" t="s">
-        <v>24</v>
-      </c>
+        <f t="shared" si="10"/>
+        <v>40</v>
+      </c>
+      <c r="F31"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32">
+        <f>B22-B19-1</f>
+        <v>514</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ref="C32:E32" si="11">C22-C19-1</f>
+        <v>628</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="11"/>
+        <v>802</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="11"/>
+        <v>1120</v>
+      </c>
+      <c r="F32"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B32">
-        <f>B31+B19</f>
-        <v>492</v>
-      </c>
-      <c r="C32">
-        <f>C31+C19</f>
-        <v>643</v>
-      </c>
-      <c r="D32">
-        <f>D31+D19</f>
-        <v>777</v>
-      </c>
-      <c r="E32">
-        <f>E31+E19</f>
-        <v>1089</v>
-      </c>
-      <c r="F32">
-        <v>1094</v>
-      </c>
-      <c r="G32" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="B33">
-        <f>B17-1</f>
-        <v>479</v>
+        <f>B22-1</f>
+        <v>524</v>
       </c>
       <c r="C33">
-        <f t="shared" ref="C33:E33" si="6">C17-1</f>
-        <v>599</v>
+        <f t="shared" ref="C33:E33" si="12">C22-1</f>
+        <v>665</v>
       </c>
       <c r="D33">
-        <f t="shared" si="6"/>
-        <v>767</v>
+        <f t="shared" si="12"/>
+        <v>805</v>
       </c>
       <c r="E33">
-        <f t="shared" si="6"/>
-        <v>1079</v>
-      </c>
-      <c r="F33">
-        <v>1079</v>
-      </c>
-      <c r="G33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="12"/>
+        <v>1124</v>
+      </c>
+      <c r="F33"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="E34"/>
       <c r="F34"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1166,58 +1086,58 @@
       </c>
       <c r="F36"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B37">
-        <f>B17/8</f>
+        <f>B18/8</f>
         <v>60</v>
       </c>
       <c r="C37">
-        <f>C17/8</f>
+        <f>C18/8</f>
         <v>75</v>
       </c>
       <c r="D37">
-        <f>D17/8</f>
+        <f>D18/8</f>
         <v>96</v>
       </c>
       <c r="E37">
-        <f>E17/8</f>
+        <f>E18/8</f>
         <v>135</v>
       </c>
       <c r="F37"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B38">
-        <f>ROUNDDOWN(B17/10,0)</f>
+        <f>ROUNDDOWN(B18/10,0)</f>
         <v>48</v>
       </c>
       <c r="C38">
-        <f>ROUNDDOWN(C17/10,0)</f>
+        <f>ROUNDDOWN(C18/10,0)</f>
         <v>60</v>
       </c>
       <c r="D38">
-        <f>ROUNDDOWN(D17/10,0)</f>
+        <f>ROUNDDOWN(D18/10,0)</f>
         <v>76</v>
       </c>
       <c r="E38">
-        <f>ROUNDDOWN(E17/10,0)</f>
+        <f>ROUNDDOWN(E18/10,0)</f>
         <v>108</v>
       </c>
       <c r="F38"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1225,42 +1145,42 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" s="6"/>
     </row>
   </sheetData>
@@ -1270,7 +1190,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1282,7 +1202,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>